<commit_message>
add new toronto eats spots shhh don't tell anyone
</commit_message>
<xml_diff>
--- a/_posts/2023-10-20-good-eatins-toronto/Eat_Data.xlsx
+++ b/_posts/2023-10-20-good-eatins-toronto/Eat_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobford/Documents/GitHub/forddataforge/_posts/2023-10-20-good-eatins-toronto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA739C8D-BD26-E045-B9EE-BAD0A82B2945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074F0078-B520-1C42-B59D-861C2C020BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="760" windowWidth="18660" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -190,6 +190,33 @@
   </si>
   <si>
     <t>Sandwiches</t>
+  </si>
+  <si>
+    <t>Leftfield Brewery</t>
+  </si>
+  <si>
+    <t>Fenway Red - really good beer</t>
+  </si>
+  <si>
+    <t>Brewery</t>
+  </si>
+  <si>
+    <t>La Banane</t>
+  </si>
+  <si>
+    <t>Trinity Bellwoods</t>
+  </si>
+  <si>
+    <t>Raw Bar, Maitake Mushroom was a sneaky star, amazing cocktails</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Lamoon Thai Café</t>
+  </si>
+  <si>
+    <t>Cuteness levels unmatched, lunch specials are great, thai tea c'mon now</t>
   </si>
 </sst>
 </file>
@@ -519,16 +546,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -834,7 +861,64 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D16" s="2"/>
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16">
+        <v>43.674216711648498</v>
+      </c>
+      <c r="F16">
+        <v>-79.330432202501399</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17">
+        <v>43.649649350878001</v>
+      </c>
+      <c r="F17">
+        <v>-79.4204187426581</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18">
+        <v>43.666404968196701</v>
+      </c>
+      <c r="F18">
+        <v>-79.348041345209097</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
lake inez - swoon
</commit_message>
<xml_diff>
--- a/_posts/2023-10-20-good-eatins-toronto/Eat_Data.xlsx
+++ b/_posts/2023-10-20-good-eatins-toronto/Eat_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobford/Documents/GitHub/forddataforge/_posts/2023-10-20-good-eatins-toronto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5195B17D-59BC-3946-BA04-067D7FB173FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114A21F1-11A4-A848-A2BE-BA9968C0C7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="760" windowWidth="18660" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -226,6 +226,15 @@
   </si>
   <si>
     <t>Malay/Singaporean</t>
+  </si>
+  <si>
+    <t>Lake Inez</t>
+  </si>
+  <si>
+    <t>Secret patio menu, really anything on the menu is going to be outrageous; as of August 2024, our favorite restaurant in Toronto</t>
+  </si>
+  <si>
+    <t>Farm to Table but also kinda Asian?</t>
   </si>
 </sst>
 </file>
@@ -555,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -949,6 +958,26 @@
         <v>-79.276638315344002</v>
       </c>
     </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20">
+        <v>43.673155291418801</v>
+      </c>
+      <c r="F20">
+        <v>-79.3208615612443</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
January 2025 clean up
</commit_message>
<xml_diff>
--- a/_posts/2023-10-20-good-eatins-toronto/Eat_Data.xlsx
+++ b/_posts/2023-10-20-good-eatins-toronto/Eat_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10119"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobford/Documents/GitHub/forddataforge/_posts/2023-10-20-good-eatins-toronto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475B49C9-CAB6-4C48-9B55-B2CD62F07BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FDEC18-A933-5349-93FD-25E766A4C32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="1220" windowWidth="22800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="113">
   <si>
     <t>Name</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Menu changes everytime. What an incredible meal, the wine was amazing as well!</t>
   </si>
   <si>
-    <t>Canadian</t>
-  </si>
-  <si>
     <t>Sunny's Chinese</t>
   </si>
   <si>
@@ -276,12 +273,6 @@
     <t>Bay-Cloverhill</t>
   </si>
   <si>
-    <t>Chongqing Chicken + Spicy Potatoes</t>
-  </si>
-  <si>
-    <t>Sichuan</t>
-  </si>
-  <si>
     <t>Ascari Enoteca</t>
   </si>
   <si>
@@ -328,6 +319,60 @@
   </si>
   <si>
     <t>Tacos, any tacos</t>
+  </si>
+  <si>
+    <t>Yummy Chinese</t>
+  </si>
+  <si>
+    <t>Popcorn chicken is wildly addictive, very reasonable price, best takeout Cantonese style Chinese</t>
+  </si>
+  <si>
+    <t>Gio Rana's Really Really Nice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giant Meatball, really anything? Killer Italian. </t>
+  </si>
+  <si>
+    <t>Enoteca Sociale</t>
+  </si>
+  <si>
+    <t>Little Portugal</t>
+  </si>
+  <si>
+    <t>Fresh pastas, mocktails were great, stunning meal</t>
+  </si>
+  <si>
+    <t>MIMI Chinese</t>
+  </si>
+  <si>
+    <t>Yorkville</t>
+  </si>
+  <si>
+    <t>Shrimp Toast was stunning, Hidden Crispy Chicken, very playful and flavorful and everything good in the world</t>
+  </si>
+  <si>
+    <t>Pho + noodle soup, cash only</t>
+  </si>
+  <si>
+    <t>Que Ling Vietnamese Cuisine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ocha's </t>
+  </si>
+  <si>
+    <t>Jerk chicken, festival; have heard great things on their oxtail but have yet to try</t>
+  </si>
+  <si>
+    <t>Chongqing Chicken + Spicy Potatoes; Sichuan goodness</t>
+  </si>
+  <si>
+    <t>Taqueria el pastorcito</t>
+  </si>
+  <si>
+    <t>Allan Gardens ish?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">al pastor! </t>
   </si>
 </sst>
 </file>
@@ -657,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -902,7 +947,7 @@
         <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E12">
         <v>43.154903513476697</v>
@@ -913,13 +958,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>45</v>
-      </c>
-      <c r="C13" t="s">
-        <v>46</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
@@ -933,13 +978,13 @@
     </row>
     <row r="14" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="D14" t="s">
         <v>29</v>
@@ -953,16 +998,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
         <v>49</v>
       </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>50</v>
-      </c>
-      <c r="D15" t="s">
-        <v>51</v>
       </c>
       <c r="E15">
         <v>43.665968364297001</v>
@@ -973,16 +1018,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
         <v>52</v>
       </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="D16" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="E16">
         <v>43.674216711648498</v>
@@ -993,16 +1038,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
         <v>55</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>56</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>57</v>
-      </c>
-      <c r="D17" t="s">
-        <v>58</v>
       </c>
       <c r="E17">
         <v>43.649649350878001</v>
@@ -1013,13 +1058,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
         <v>59</v>
-      </c>
-      <c r="B18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" t="s">
-        <v>60</v>
       </c>
       <c r="D18" t="s">
         <v>23</v>
@@ -1033,16 +1078,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
       </c>
       <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" t="s">
         <v>62</v>
-      </c>
-      <c r="D19" t="s">
-        <v>63</v>
       </c>
       <c r="E19">
         <v>43.787934054235997</v>
@@ -1053,13 +1098,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
         <v>64</v>
-      </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>65</v>
       </c>
       <c r="D20" t="s">
         <v>33</v>
@@ -1073,16 +1118,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
         <v>66</v>
       </c>
-      <c r="B21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>67</v>
-      </c>
-      <c r="D21" t="s">
-        <v>68</v>
       </c>
       <c r="E21">
         <v>43.645564856373603</v>
@@ -1093,13 +1138,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
         <v>69</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>70</v>
-      </c>
-      <c r="C22" t="s">
-        <v>71</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
@@ -1113,13 +1158,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" t="s">
         <v>72</v>
-      </c>
-      <c r="B23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" t="s">
-        <v>73</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
@@ -1133,13 +1178,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
         <v>74</v>
-      </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" t="s">
-        <v>75</v>
       </c>
       <c r="D24" t="s">
         <v>33</v>
@@ -1153,13 +1198,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
         <v>76</v>
-      </c>
-      <c r="B25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" t="s">
-        <v>77</v>
       </c>
       <c r="D25" t="s">
         <v>33</v>
@@ -1173,16 +1218,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" t="s">
         <v>78</v>
       </c>
-      <c r="B26" t="s">
-        <v>79</v>
-      </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>4</v>
       </c>
       <c r="E26">
         <v>43.6680065985109</v>
@@ -1193,13 +1238,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D27" t="s">
         <v>38</v>
@@ -1213,13 +1258,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
@@ -1233,16 +1278,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
         <v>85</v>
       </c>
-      <c r="C29" t="s">
-        <v>88</v>
-      </c>
       <c r="D29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E29">
         <v>43.677749263445399</v>
@@ -1253,16 +1298,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D30" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E30">
         <v>43.659137099857602</v>
@@ -1273,16 +1318,16 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D31" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E31">
         <v>43.664087346217997</v>
@@ -1293,22 +1338,162 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D32" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E32">
         <v>43.654592951484197</v>
       </c>
       <c r="F32">
         <v>-79.400673061407602</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>43.670188149640403</v>
+      </c>
+      <c r="F33">
+        <v>-79.336298702573899</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34">
+        <v>43.663396670633396</v>
+      </c>
+      <c r="F34">
+        <v>-79.330474179261202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35">
+        <v>43.649780159325701</v>
+      </c>
+      <c r="F35">
+        <v>-79.425617316722807</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <v>43.674636892456697</v>
+      </c>
+      <c r="F36">
+        <v>-79.3981557604356</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>105</v>
+      </c>
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37">
+        <v>43.665957195598601</v>
+      </c>
+      <c r="F37">
+        <v>-79.349426857565504</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38">
+        <v>43.661691129281799</v>
+      </c>
+      <c r="F38">
+        <v>-79.338724543548807</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>110</v>
+      </c>
+      <c r="B39" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D39" t="s">
+        <v>92</v>
+      </c>
+      <c r="E39">
+        <v>43.664608478470498</v>
+      </c>
+      <c r="F39">
+        <v>-79.384586629285295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>